<commit_message>
tamburu... remove the excel sheet
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -1,38 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tabualrob\git\CBISmoke\src\com\generic\config\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C35AF2D-AAC5-440F-B911-E14D1D7015C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="SetupBrowsers" sheetId="1" r:id="rId1"/>
-    <sheet name="SetupRunners" sheetId="2" r:id="rId2"/>
-    <sheet name="Brands" sheetId="3" r:id="rId3"/>
-    <sheet name="Envs" sheetId="4" r:id="rId4"/>
-    <sheet name="SmkRegression" sheetId="5" r:id="rId5"/>
-    <sheet name="HomePageRegression" sheetId="6" r:id="rId6"/>
-    <sheet name="CLPRegression" sheetId="7" r:id="rId7"/>
-    <sheet name="CheckOutRegression" sheetId="8" r:id="rId8"/>
-    <sheet name="PayPalCheckOutRegression" sheetId="9" r:id="rId9"/>
-    <sheet name="PDPRegression" sheetId="10" r:id="rId10"/>
-    <sheet name="CartRegression" sheetId="11" r:id="rId11"/>
-    <sheet name="PLPRegression" sheetId="12" r:id="rId12"/>
-    <sheet name="RegistrationRegression" sheetId="13" r:id="rId13"/>
-    <sheet name="LoginRegression" sheetId="14" r:id="rId14"/>
-    <sheet name="GiftRegistryRegression" sheetId="15" r:id="rId15"/>
-    <sheet name="users" sheetId="16" r:id="rId16"/>
-    <sheet name="addresses" sheetId="17" r:id="rId17"/>
-    <sheet name="cards" sheetId="18" r:id="rId18"/>
+    <sheet state="visible" name="SetupBrowsers" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="SetupRunners" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Brands" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Envs" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="SmkRegression" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="HomePageRegression" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="CLPRegression" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="CheckOutRegression" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="PayPalCheckOutRegression" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="PDPRegression" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="CartRegression" sheetId="11" r:id="rId14"/>
+    <sheet state="visible" name="PLPRegression" sheetId="12" r:id="rId15"/>
+    <sheet state="visible" name="RegistrationRegression" sheetId="13" r:id="rId16"/>
+    <sheet state="visible" name="LoginRegression" sheetId="14" r:id="rId17"/>
+    <sheet state="visible" name="GiftRegistryRegression" sheetId="15" r:id="rId18"/>
+    <sheet state="visible" name="users" sheetId="16" r:id="rId19"/>
+    <sheet state="visible" name="addresses" sheetId="17" r:id="rId20"/>
+    <sheet state="visible" name="cards" sheetId="18" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId22" roundtripDataSignature="AMtx7mhN/Rga5XRgXxcnRjWWIXJyLDf17A=="/>
@@ -42,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="285">
   <si>
     <t>Regression</t>
   </si>
@@ -1027,63 +1018,63 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <fonts count="11">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="0"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arimo"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arimo"/>
     </font>
@@ -1093,7 +1084,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1121,13 +1112,7 @@
     </fill>
   </fills>
   <borders count="15">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FFFFFFFF"/>
@@ -1138,19 +1123,14 @@
       <top style="thin">
         <color rgb="FFFFFFFF"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
         <color rgb="FFFFFFFF"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1163,7 +1143,6 @@
         <color theme="0"/>
       </top>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1178,7 +1157,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1193,7 +1171,6 @@
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1202,11 +1179,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1218,19 +1193,14 @@
       <top style="thin">
         <color theme="0"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1245,7 +1215,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -1258,27 +1227,19 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1287,9 +1248,6 @@
       <right style="thin">
         <color rgb="FFFFFFFF"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1300,299 +1258,371 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="97">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="11" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="11" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="13" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="12" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="7" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="14" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="4" fillId="0" fontId="10" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1782,27 +1812,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF632423"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="7.875" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="13.5"/>
+    <col customWidth="1" min="2" max="2" width="7.88"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1810,48 +1838,50 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="8"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4">
       <c r="A4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF205867"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="7.25" customWidth="1"/>
-    <col min="2" max="2" width="6.75" customWidth="1"/>
-    <col min="3" max="3" width="42.75" customWidth="1"/>
-    <col min="4" max="5" width="18.625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="7.25"/>
+    <col customWidth="1" min="2" max="2" width="6.75"/>
+    <col customWidth="1" min="3" max="3" width="42.75"/>
+    <col customWidth="1" min="4" max="5" width="18.63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="41" t="s">
         <v>23</v>
       </c>
@@ -1868,7 +1898,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2">
       <c r="A2" s="20" t="s">
         <v>94</v>
       </c>
@@ -1883,7 +1913,7 @@
       </c>
       <c r="E2" s="46"/>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3">
       <c r="A3" s="47" t="s">
         <v>97</v>
       </c>
@@ -1900,7 +1930,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4">
       <c r="A4" s="47" t="s">
         <v>97</v>
       </c>
@@ -1917,7 +1947,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5">
       <c r="A5" s="22" t="s">
         <v>105</v>
       </c>
@@ -1933,29 +1963,31 @@
       <c r="E5" s="50"/>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF205867"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="5.75" customWidth="1"/>
-    <col min="2" max="2" width="6.75" customWidth="1"/>
-    <col min="3" max="3" width="45.375" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="5.75"/>
+    <col customWidth="1" min="2" max="2" width="6.75"/>
+    <col customWidth="1" min="3" max="3" width="45.38"/>
+    <col customWidth="1" min="4" max="4" width="20.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1">
       <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
@@ -1969,7 +2001,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.25" customHeight="1">
+    <row r="2" ht="20.25" customHeight="1">
       <c r="A2" s="49" t="s">
         <v>101</v>
       </c>
@@ -1982,30 +2014,30 @@
       <c r="D2" s="53"/>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF205867"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="18.75" customWidth="1"/>
-    <col min="4" max="4" width="54.875" customWidth="1"/>
+    <col customWidth="1" min="1" max="2" width="8.0"/>
+    <col customWidth="1" min="3" max="3" width="18.75"/>
+    <col customWidth="1" min="4" max="4" width="54.88"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="19" t="s">
         <v>23</v>
       </c>
@@ -2019,7 +2051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
+    <row r="2">
       <c r="A2" s="20" t="s">
         <v>109</v>
       </c>
@@ -2031,13 +2063,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1">
+    <row r="3">
       <c r="A3" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>6</v>
-      </c>
+      <c r="B3" s="20"/>
       <c r="C3" s="52" t="s">
         <v>114</v>
       </c>
@@ -2045,11 +2075,13 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1">
+    <row r="4">
       <c r="A4" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="20" t="s">
+        <v>6</v>
+      </c>
       <c r="C4" s="52" t="s">
         <v>117</v>
       </c>
@@ -2057,11 +2089,13 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5">
       <c r="A5" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="60"/>
+      <c r="B5" s="60" t="s">
+        <v>6</v>
+      </c>
       <c r="C5" s="62" t="s">
         <v>125</v>
       </c>
@@ -2070,30 +2104,32 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF205867"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="32.75" customWidth="1"/>
-    <col min="4" max="4" width="12.125" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="62.125" customWidth="1"/>
+    <col customWidth="1" min="1" max="2" width="8.0"/>
+    <col customWidth="1" min="3" max="3" width="32.75"/>
+    <col customWidth="1" min="4" max="4" width="12.13"/>
+    <col customWidth="1" min="5" max="5" width="11.0"/>
+    <col customWidth="1" min="6" max="6" width="62.13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="54" t="s">
         <v>23</v>
       </c>
@@ -2113,7 +2149,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2" s="27" t="s">
         <v>122</v>
       </c>
@@ -2133,7 +2169,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
+    <row r="3">
       <c r="A3" s="51" t="s">
         <v>131</v>
       </c>
@@ -2152,30 +2188,32 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF205867"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="29.125" customWidth="1"/>
-    <col min="4" max="4" width="26.625" customWidth="1"/>
-    <col min="5" max="5" width="5.25" customWidth="1"/>
-    <col min="6" max="6" width="60.75" customWidth="1"/>
+    <col customWidth="1" min="1" max="2" width="8.0"/>
+    <col customWidth="1" min="3" max="3" width="29.13"/>
+    <col customWidth="1" min="4" max="4" width="26.63"/>
+    <col customWidth="1" min="5" max="5" width="5.25"/>
+    <col customWidth="1" min="6" max="6" width="60.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1">
       <c r="A1" s="58" t="s">
         <v>23</v>
       </c>
@@ -2195,7 +2233,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2" s="66" t="s">
         <v>124</v>
       </c>
@@ -2213,7 +2251,7 @@
       </c>
       <c r="F2" s="74"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3" s="66" t="s">
         <v>145</v>
       </c>
@@ -2231,7 +2269,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="53" t="s">
         <v>159</v>
       </c>
@@ -2249,7 +2287,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.5">
+    <row r="5">
       <c r="A5" s="36" t="s">
         <v>165</v>
       </c>
@@ -2265,7 +2303,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6" s="84" t="s">
         <v>169</v>
       </c>
@@ -2282,27 +2320,28 @@
       <c r="F6" s="92"/>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF205867"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="9" max="9" width="49.75" customWidth="1"/>
+    <col customWidth="1" min="9" max="9" width="49.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1">
       <c r="A1" s="69" t="s">
         <v>23</v>
       </c>
@@ -2331,7 +2370,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.5" customHeight="1">
+    <row r="2" ht="28.5" customHeight="1">
       <c r="A2" s="80" t="s">
         <v>158</v>
       </c>
@@ -2351,16 +2390,16 @@
         <v>171</v>
       </c>
       <c r="G2" s="80">
-        <v>12</v>
+        <v>12.0</v>
       </c>
       <c r="H2" s="80">
-        <v>2025</v>
+        <v>2025.0</v>
       </c>
       <c r="I2" s="80" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.5" customHeight="1">
+    <row r="3" ht="28.5" customHeight="1">
       <c r="A3" s="89" t="s">
         <v>174</v>
       </c>
@@ -2378,41 +2417,41 @@
         <v>171</v>
       </c>
       <c r="G3" s="80">
-        <v>12</v>
+        <v>12.0</v>
       </c>
       <c r="H3" s="80">
-        <v>2025</v>
+        <v>2025.0</v>
       </c>
       <c r="I3" s="80" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF002060"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="5.25" customWidth="1"/>
-    <col min="2" max="2" width="4.125" customWidth="1"/>
-    <col min="3" max="3" width="8.875" customWidth="1"/>
-    <col min="4" max="4" width="8.625" customWidth="1"/>
-    <col min="5" max="5" width="8.25" customWidth="1"/>
-    <col min="6" max="6" width="10.75" customWidth="1"/>
-    <col min="7" max="7" width="23.375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="5.25"/>
+    <col customWidth="1" min="2" max="2" width="4.13"/>
+    <col customWidth="1" min="3" max="3" width="8.88"/>
+    <col customWidth="1" min="4" max="4" width="8.63"/>
+    <col customWidth="1" min="5" max="5" width="8.25"/>
+    <col customWidth="1" min="6" max="6" width="10.75"/>
+    <col customWidth="1" min="7" max="7" width="23.38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1">
       <c r="A1" s="58" t="s">
         <v>139</v>
       </c>
@@ -2435,7 +2474,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2">
       <c r="A2" s="59" t="s">
         <v>138</v>
       </c>
@@ -2458,7 +2497,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3">
       <c r="A3" s="59" t="s">
         <v>173</v>
       </c>
@@ -2481,7 +2520,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4">
       <c r="A4" s="59" t="s">
         <v>67</v>
       </c>
@@ -2504,7 +2543,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5">
       <c r="A5" s="59" t="s">
         <v>179</v>
       </c>
@@ -2527,7 +2566,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6">
       <c r="A6" s="59" t="s">
         <v>182</v>
       </c>
@@ -2550,7 +2589,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7">
       <c r="A7" s="59" t="s">
         <v>184</v>
       </c>
@@ -2573,7 +2612,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8">
       <c r="A8" s="59" t="s">
         <v>186</v>
       </c>
@@ -2596,7 +2635,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9">
       <c r="A9" s="59" t="s">
         <v>189</v>
       </c>
@@ -2619,7 +2658,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10">
       <c r="A10" s="59" t="s">
         <v>191</v>
       </c>
@@ -2642,7 +2681,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11">
       <c r="A11" s="59" t="s">
         <v>201</v>
       </c>
@@ -2665,7 +2704,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12">
       <c r="A12" s="59" t="s">
         <v>208</v>
       </c>
@@ -2688,7 +2727,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13">
       <c r="A13" s="59" t="s">
         <v>216</v>
       </c>
@@ -2711,7 +2750,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14">
       <c r="A14" s="59" t="s">
         <v>48</v>
       </c>
@@ -2734,7 +2773,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15">
       <c r="A15" s="59" t="s">
         <v>234</v>
       </c>
@@ -2757,7 +2796,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16">
       <c r="A16" s="59" t="s">
         <v>153</v>
       </c>
@@ -2780,7 +2819,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17">
       <c r="A17" s="59" t="s">
         <v>249</v>
       </c>
@@ -2803,7 +2842,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18">
       <c r="A18" s="59" t="s">
         <v>253</v>
       </c>
@@ -2826,7 +2865,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19">
       <c r="A19" s="59" t="s">
         <v>255</v>
       </c>
@@ -2849,7 +2888,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20">
       <c r="A20" s="59" t="s">
         <v>257</v>
       </c>
@@ -2872,7 +2911,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="59" t="s">
         <v>259</v>
       </c>
@@ -2895,7 +2934,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="59" t="s">
         <v>261</v>
       </c>
@@ -2918,7 +2957,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="59" t="s">
         <v>263</v>
       </c>
@@ -2941,7 +2980,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="59" t="s">
         <v>265</v>
       </c>
@@ -2964,7 +3003,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="59" t="s">
         <v>267</v>
       </c>
@@ -2987,7 +3026,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="59" t="s">
         <v>269</v>
       </c>
@@ -3010,7 +3049,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="59" t="s">
         <v>271</v>
       </c>
@@ -3033,7 +3072,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1">
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="59" t="s">
         <v>273</v>
       </c>
@@ -3056,7 +3095,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="59" t="s">
         <v>275</v>
       </c>
@@ -3079,7 +3118,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="59" t="s">
         <v>277</v>
       </c>
@@ -3102,7 +3141,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="59" t="s">
         <v>279</v>
       </c>
@@ -3125,7 +3164,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="59" t="s">
         <v>281</v>
       </c>
@@ -3148,7 +3187,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1">
+    <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="59" t="s">
         <v>283</v>
       </c>
@@ -3173,34 +3212,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G33" r:id="rId1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink r:id="rId1" ref="G33"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF002060"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.875" customWidth="1"/>
-    <col min="3" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="17.75" customWidth="1"/>
-    <col min="6" max="6" width="9.125" customWidth="1"/>
-    <col min="7" max="7" width="8.75" customWidth="1"/>
-    <col min="8" max="8" width="14.875" customWidth="1"/>
-    <col min="9" max="9" width="10.75" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="10.88"/>
+    <col customWidth="1" min="3" max="4" width="10.5"/>
+    <col customWidth="1" min="5" max="5" width="17.75"/>
+    <col customWidth="1" min="6" max="6" width="9.13"/>
+    <col customWidth="1" min="7" max="7" width="8.75"/>
+    <col customWidth="1" min="8" max="8" width="14.88"/>
+    <col customWidth="1" min="9" max="9" width="10.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="43" t="s">
         <v>187</v>
       </c>
@@ -3229,7 +3270,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2">
       <c r="A2" s="61" t="s">
         <v>209</v>
       </c>
@@ -3258,7 +3299,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3">
       <c r="A3" s="61" t="s">
         <v>227</v>
       </c>
@@ -3287,7 +3328,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4">
       <c r="A4" s="61" t="s">
         <v>47</v>
       </c>
@@ -3316,7 +3357,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5">
       <c r="A5" s="61" t="s">
         <v>247</v>
       </c>
@@ -3346,31 +3387,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF002060"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="15.375" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="9.625" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="9.875" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="10.0"/>
+    <col customWidth="1" min="2" max="2" width="15.38"/>
+    <col customWidth="1" min="3" max="3" width="11.5"/>
+    <col customWidth="1" min="4" max="4" width="9.63"/>
+    <col customWidth="1" min="5" max="5" width="11.5"/>
+    <col customWidth="1" min="6" max="6" width="9.88"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="43" t="s">
         <v>192</v>
       </c>
@@ -3390,7 +3433,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2" s="61" t="s">
         <v>43</v>
       </c>
@@ -3410,7 +3453,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3" s="61" t="s">
         <v>212</v>
       </c>
@@ -3430,7 +3473,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4" s="61" t="s">
         <v>219</v>
       </c>
@@ -3450,7 +3493,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5" s="61" t="s">
         <v>228</v>
       </c>
@@ -3470,7 +3513,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6" s="61" t="s">
         <v>235</v>
       </c>
@@ -3490,7 +3533,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
@@ -3498,7 +3541,7 @@
         <v>240</v>
       </c>
       <c r="C7" s="6">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D7" s="61" t="s">
         <v>41</v>
@@ -3511,27 +3554,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF632423"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="22.375" customWidth="1"/>
-    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="22.38"/>
+    <col customWidth="1" min="2" max="2" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3539,7 +3584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -3547,7 +3592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -3555,7 +3600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -3563,7 +3608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -3571,7 +3616,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -3579,7 +3624,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -3587,7 +3632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -3595,7 +3640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -3603,7 +3648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -3611,7 +3656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
@@ -3620,24 +3665,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF632423"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3645,7 +3691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -3653,7 +3699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -3661,42 +3707,41 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="9"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="9"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6">
       <c r="A6" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="9"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF632423"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -3704,7 +3749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -3712,7 +3757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3">
       <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
@@ -3720,7 +3765,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4">
       <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
@@ -3729,28 +3774,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF205867"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="7.875" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="10" width="18" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="7.88"/>
+    <col customWidth="1" min="2" max="2" width="8.0"/>
+    <col customWidth="1" min="3" max="3" width="34.0"/>
+    <col customWidth="1" min="4" max="10" width="18.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="12" t="s">
         <v>23</v>
       </c>
@@ -3782,7 +3827,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1">
+    <row r="2">
       <c r="A2" s="17" t="s">
         <v>36</v>
       </c>
@@ -3815,29 +3860,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF205867"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="7.875" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="55.25" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="7.88"/>
+    <col customWidth="1" min="2" max="2" width="8.0"/>
+    <col customWidth="1" min="3" max="3" width="55.25"/>
+    <col customWidth="1" min="4" max="4" width="18.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="12" t="s">
         <v>23</v>
       </c>
@@ -3851,7 +3898,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
+    <row r="2">
       <c r="A2" s="18" t="s">
         <v>37</v>
       </c>
@@ -3865,7 +3912,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1">
+    <row r="3">
       <c r="A3" s="18" t="s">
         <v>50</v>
       </c>
@@ -3879,7 +3926,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1">
+    <row r="4">
       <c r="A4" s="18" t="s">
         <v>52</v>
       </c>
@@ -3891,7 +3938,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1">
+    <row r="5">
       <c r="A5" s="18" t="s">
         <v>56</v>
       </c>
@@ -3903,7 +3950,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1">
+    <row r="6">
       <c r="A6" s="18" t="s">
         <v>62</v>
       </c>
@@ -3915,7 +3962,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1">
+    <row r="7">
       <c r="A7" s="18" t="s">
         <v>66</v>
       </c>
@@ -3927,7 +3974,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="240">
+    <row r="8">
       <c r="A8" s="18" t="s">
         <v>70</v>
       </c>
@@ -3939,7 +3986,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1">
+    <row r="9">
       <c r="A9" s="18" t="s">
         <v>78</v>
       </c>
@@ -3953,7 +4000,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1">
+    <row r="10">
       <c r="A10" s="39" t="s">
         <v>82</v>
       </c>
@@ -3965,7 +4012,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1">
+    <row r="11">
       <c r="A11" s="39" t="s">
         <v>90</v>
       </c>
@@ -3978,27 +4025,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF205867"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="3" max="3" width="37.375" customWidth="1"/>
+    <col customWidth="1" min="3" max="3" width="37.38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="19" t="s">
         <v>23</v>
       </c>
@@ -4012,7 +4060,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="85.5">
+    <row r="2">
       <c r="A2" s="17" t="s">
         <v>39</v>
       </c>
@@ -4027,33 +4075,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF205867"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="2" width="7.875" customWidth="1"/>
-    <col min="3" max="3" width="24.5" customWidth="1"/>
-    <col min="4" max="4" width="20.75" customWidth="1"/>
-    <col min="5" max="5" width="13.625" customWidth="1"/>
-    <col min="6" max="6" width="17.375" customWidth="1"/>
-    <col min="7" max="7" width="11.875" customWidth="1"/>
-    <col min="8" max="8" width="13.875" customWidth="1"/>
-    <col min="9" max="9" width="12.125" customWidth="1"/>
-    <col min="10" max="10" width="17.25" customWidth="1"/>
+    <col customWidth="1" min="1" max="2" width="7.88"/>
+    <col customWidth="1" min="3" max="3" width="24.5"/>
+    <col customWidth="1" min="4" max="4" width="20.75"/>
+    <col customWidth="1" min="5" max="5" width="13.63"/>
+    <col customWidth="1" min="6" max="6" width="17.38"/>
+    <col customWidth="1" min="7" max="7" width="11.88"/>
+    <col customWidth="1" min="8" max="8" width="13.88"/>
+    <col customWidth="1" min="9" max="9" width="12.13"/>
+    <col customWidth="1" min="10" max="10" width="17.25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="12" t="s">
         <v>23</v>
       </c>
@@ -4085,7 +4133,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1">
+    <row r="2">
       <c r="A2" s="17" t="s">
         <v>53</v>
       </c>
@@ -4117,7 +4165,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1">
+    <row r="3">
       <c r="A3" s="17" t="s">
         <v>71</v>
       </c>
@@ -4131,7 +4179,7 @@
         <v>75</v>
       </c>
       <c r="E3" s="17">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>42</v>
@@ -4149,7 +4197,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1">
+    <row r="4">
       <c r="A4" s="17" t="s">
         <v>81</v>
       </c>
@@ -4181,7 +4229,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1">
+    <row r="5">
       <c r="A5" s="17" t="s">
         <v>87</v>
       </c>
@@ -4195,7 +4243,7 @@
         <v>89</v>
       </c>
       <c r="E5" s="17">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>42</v>
@@ -4214,30 +4262,32 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <tabColor rgb="FF205867"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="2" width="7.875" customWidth="1"/>
-    <col min="3" max="3" width="24.5" customWidth="1"/>
-    <col min="4" max="4" width="20.75" customWidth="1"/>
-    <col min="5" max="6" width="11.875" customWidth="1"/>
-    <col min="7" max="7" width="17.25" customWidth="1"/>
+    <col customWidth="1" min="1" max="2" width="7.88"/>
+    <col customWidth="1" min="3" max="3" width="24.5"/>
+    <col customWidth="1" min="4" max="4" width="20.75"/>
+    <col customWidth="1" min="5" max="6" width="11.88"/>
+    <col customWidth="1" min="7" max="7" width="17.25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1">
+    <row r="1">
       <c r="A1" s="12" t="s">
         <v>23</v>
       </c>
@@ -4260,7 +4310,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1">
+    <row r="2">
       <c r="A2" s="17" t="s">
         <v>53</v>
       </c>
@@ -4283,7 +4333,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1">
+    <row r="3">
       <c r="A3" s="17" t="s">
         <v>71</v>
       </c>
@@ -4297,7 +4347,7 @@
         <v>76</v>
       </c>
       <c r="E3" s="17">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="F3" s="35" t="s">
         <v>17</v>
@@ -4305,7 +4355,9 @@
       <c r="G3" s="36"/>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>